<commit_message>
added total profit and losses
</commit_message>
<xml_diff>
--- a/trading_data/total_pl.xlsx
+++ b/trading_data/total_pl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Desktop\trade_analysis\trading_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63C2E4-7D4D-4A90-8B45-D64B015DBB17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CFE0C2-D2AA-4AB8-B5CB-89A36C08FB34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="3540" windowWidth="21600" windowHeight="11385" xr2:uid="{74563E13-67B1-478E-A46B-1DAF4D8296CF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74563E13-67B1-478E-A46B-1DAF4D8296CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +71,9 @@
   </si>
   <si>
     <t>Monthly_pl</t>
+  </si>
+  <si>
+    <t>number of trades taken</t>
   </si>
 </sst>
 </file>
@@ -126,12 +128,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -447,23 +450,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CEB993-576A-4484-943F-5B7E4DB00662}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,12 +490,15 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43964</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1500</v>
       </c>
       <c r="C2" s="2">
@@ -510,12 +518,15 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43965</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <f t="shared" ref="B3:B22" si="1">D2</f>
         <v>1479</v>
       </c>
@@ -536,12 +547,15 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43966</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <f t="shared" si="1"/>
         <v>1482.43</v>
       </c>
@@ -562,12 +576,15 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43970</v>
-      </c>
-      <c r="B5">
+        <v>43969</v>
+      </c>
+      <c r="B5" s="5">
         <f t="shared" si="1"/>
         <v>1459.02</v>
       </c>
@@ -588,12 +605,15 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43971</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <f t="shared" si="1"/>
         <v>1527.02</v>
       </c>
@@ -614,12 +634,15 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43972</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <f t="shared" si="1"/>
         <v>1627.27</v>
       </c>
@@ -640,12 +663,15 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43977</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <f t="shared" si="1"/>
         <v>1638.02</v>
       </c>
@@ -666,12 +692,15 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43979</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <f t="shared" si="1"/>
         <v>1611.52</v>
       </c>
@@ -692,12 +721,15 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43973</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <f t="shared" si="1"/>
         <v>1598.2</v>
       </c>
@@ -718,12 +750,15 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43983</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <f t="shared" si="1"/>
         <v>1639.02</v>
       </c>
@@ -744,12 +779,15 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43984</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <f t="shared" si="1"/>
         <v>1384.02</v>
       </c>
@@ -770,12 +808,15 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43985</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f t="shared" si="1"/>
         <v>1125.92</v>
       </c>
@@ -796,12 +837,15 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43986</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <f t="shared" si="1"/>
         <v>1100.92</v>
       </c>
@@ -822,12 +866,15 @@
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43987</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <f t="shared" si="1"/>
         <v>1143.1300000000001</v>
       </c>
@@ -848,12 +895,15 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43990</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <f t="shared" si="1"/>
         <v>1258.44</v>
       </c>
@@ -874,12 +924,15 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43991</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <f t="shared" si="1"/>
         <v>1247.94</v>
       </c>
@@ -900,12 +953,15 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43986</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <f t="shared" si="1"/>
         <v>1244.94</v>
       </c>
@@ -926,12 +982,15 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43993</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <f t="shared" si="1"/>
         <v>1278.78</v>
       </c>
@@ -952,12 +1011,15 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43992</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <f t="shared" si="1"/>
         <v>1296.0899999999999</v>
       </c>
@@ -978,12 +1040,15 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43993</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <f t="shared" si="1"/>
         <v>1246.47</v>
       </c>
@@ -1004,12 +1069,15 @@
       <c r="G21">
         <v>1119.01</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43994</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <f t="shared" si="1"/>
         <v>1119.01</v>
       </c>
@@ -1030,12 +1098,15 @@
       <c r="G22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43997</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>1147.51</v>
       </c>
       <c r="C23" s="2">
@@ -1055,12 +1126,15 @@
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43998</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>1154.01</v>
       </c>
       <c r="C24" s="2">
@@ -1080,13 +1154,16 @@
       <c r="G24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44046</v>
       </c>
-      <c r="B25">
-        <f>B24+C24</f>
+      <c r="B25" s="5">
+        <f t="shared" ref="B25:B31" si="2">B24+C24</f>
         <v>1107.7</v>
       </c>
       <c r="C25" s="2">
@@ -1106,56 +1183,182 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44049</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" si="2"/>
+        <v>1044.42</v>
+      </c>
+      <c r="C26" s="2">
+        <v>-16.89</v>
+      </c>
+      <c r="D26">
+        <f>C26+B26</f>
+        <v>1027.53</v>
+      </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C26)</f>
+        <v>-322.47000000000003</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44050</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="2"/>
+        <v>1027.53</v>
+      </c>
+      <c r="C27" s="2">
+        <v>-63.89</v>
+      </c>
+      <c r="D27">
+        <f>C27+B27</f>
+        <v>963.64</v>
+      </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C27)</f>
+        <v>-386.36</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44005</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" si="2"/>
+        <v>963.64</v>
+      </c>
+      <c r="C28" s="2">
+        <v>38.28</v>
+      </c>
+      <c r="D28">
+        <f>C28+B28</f>
+        <v>1001.92</v>
+      </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C28)</f>
+        <v>-348.08000000000004</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44006</v>
+      </c>
+      <c r="B29" s="5">
+        <f t="shared" si="2"/>
+        <v>1001.92</v>
+      </c>
+      <c r="C29" s="2">
+        <v>-26.68</v>
+      </c>
+      <c r="D29">
+        <f>C29+B29</f>
+        <v>975.24</v>
+      </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C29)</f>
+        <v>-374.76000000000005</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44008</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" si="2"/>
+        <v>975.24</v>
+      </c>
+      <c r="C30" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D30">
+        <f>C30+B30</f>
+        <v>995.34</v>
+      </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C30)</f>
+        <v>-354.66</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44011</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" si="2"/>
+        <v>995.34</v>
+      </c>
+      <c r="C31" s="2">
+        <v>-56.55</v>
+      </c>
+      <c r="D31">
+        <f>C31+B31</f>
+        <v>938.79000000000008</v>
+      </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C2:C31)</f>
+        <v>-411.21000000000004</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>0</v>
       </c>
@@ -1241,37 +1444,231 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C25">
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E21">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E41">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B24 B31:B1048576">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E42">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B25 B31:B1048576">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B26 B31:B1048576">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B28 B31:B1048576">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B12">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E21">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B21">
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1283,29 +1680,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E41">
+  <conditionalFormatting sqref="B29">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B24 B27:B1048576">
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1317,47 +1712,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="B30">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E42">
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B25 B27:B1048576">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
deleted a lot of ABCD's
</commit_message>
<xml_diff>
--- a/trading_data/total_pl.xlsx
+++ b/trading_data/total_pl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Desktop\trade_analysis\trading_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AABE1-427C-4BAC-AD01-AC2AE7211B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6668145A-CD5D-49D0-9131-587805052B32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74563E13-67B1-478E-A46B-1DAF4D8296CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74563E13-67B1-478E-A46B-1DAF4D8296CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CEB993-576A-4484-943F-5B7E4DB00662}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,14 +1163,14 @@
         <v>44046</v>
       </c>
       <c r="B25" s="5">
-        <f t="shared" ref="B25:B31" si="2">B24+C24</f>
+        <f t="shared" ref="B25:B32" si="2">B24+C24</f>
         <v>1107.7</v>
       </c>
       <c r="C25" s="2">
         <v>-63.28</v>
       </c>
       <c r="D25">
-        <f>C25+B25</f>
+        <f t="shared" ref="D25:D32" si="3">C25+B25</f>
         <v>1044.42</v>
       </c>
       <c r="E25">
@@ -1199,7 +1199,7 @@
         <v>-16.89</v>
       </c>
       <c r="D26">
-        <f>C26+B26</f>
+        <f t="shared" si="3"/>
         <v>1027.53</v>
       </c>
       <c r="E26">
@@ -1228,7 +1228,7 @@
         <v>-63.89</v>
       </c>
       <c r="D27">
-        <f>C27+B27</f>
+        <f t="shared" si="3"/>
         <v>963.64</v>
       </c>
       <c r="E27">
@@ -1257,7 +1257,7 @@
         <v>38.28</v>
       </c>
       <c r="D28">
-        <f>C28+B28</f>
+        <f t="shared" si="3"/>
         <v>1001.92</v>
       </c>
       <c r="E28">
@@ -1286,7 +1286,7 @@
         <v>-26.68</v>
       </c>
       <c r="D29">
-        <f>C29+B29</f>
+        <f t="shared" si="3"/>
         <v>975.24</v>
       </c>
       <c r="E29">
@@ -1312,7 +1312,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="D30">
-        <f>C30+B30</f>
+        <f t="shared" si="3"/>
         <v>995.34</v>
       </c>
       <c r="E30">
@@ -1341,7 +1341,7 @@
         <v>-56.55</v>
       </c>
       <c r="D31">
-        <f>C31+B31</f>
+        <f t="shared" si="3"/>
         <v>938.79000000000008</v>
       </c>
       <c r="E31">
@@ -1359,11 +1359,32 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B32" s="5">
+        <f t="shared" si="2"/>
+        <v>938.79000000000008</v>
+      </c>
+      <c r="C32" s="2">
+        <v>-57</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>881.79000000000008</v>
+      </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <f>SUM(C2:C32)</f>
+        <v>-468.21000000000004</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
@@ -1444,7 +1465,49 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C31">
+  <conditionalFormatting sqref="C2:C32">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E21">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E41">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -1453,6 +1516,8 @@
         <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -1464,83 +1529,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E21">
+  <conditionalFormatting sqref="B1:B24 B31:B1048576">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E41">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B24 B31:B1048576">
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E42">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B25 B31:B1048576">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B26 B31:B1048576">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E42">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -1552,7 +1609,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B25 B31:B1048576">
+  <conditionalFormatting sqref="B28">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -1564,31 +1621,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B26 B31:B1048576">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
+  <conditionalFormatting sqref="B1:B28 B31:B1048576">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -1599,19 +1632,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B28 B31:B1048576">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1621,18 +1642,54 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1644,54 +1701,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="B29">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1701,7 +1722,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1713,17 +1734,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1745,6 +1766,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1756,7 +1809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
+  <conditionalFormatting sqref="B32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>